<commit_message>
Cập nhật biên bản họp nhóm
Thay đổi các yêu cầu
</commit_message>
<xml_diff>
--- a/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
+++ b/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10668"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10668" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="20-9" sheetId="1" r:id="rId1"/>
+    <sheet name="16-10" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>Dự phòng</t>
   </si>
@@ -41,9 +42,6 @@
     <t>Thích ứng</t>
   </si>
   <si>
-    <t>Database -&gt; SQL 2005</t>
-  </si>
-  <si>
     <t>Linux</t>
   </si>
   <si>
@@ -53,9 +51,6 @@
     <t>Mục thống kê</t>
   </si>
   <si>
-    <t>Đăng nhập không đúng cho một số account</t>
-  </si>
-  <si>
     <t>Hoàn thiện</t>
   </si>
   <si>
@@ -108,13 +103,43 @@
   </si>
   <si>
     <t>TT</t>
+  </si>
+  <si>
+    <t>Database -&gt; Oracle</t>
+  </si>
+  <si>
+    <t>Giao diện mobile</t>
+  </si>
+  <si>
+    <t>Phân quyền</t>
+  </si>
+  <si>
+    <t>Quản lý đơn vị</t>
+  </si>
+  <si>
+    <t>Cập nhật máy biến áp</t>
+  </si>
+  <si>
+    <t>Cập nhật tình trạng biến áp</t>
+  </si>
+  <si>
+    <t>Phuong</t>
+  </si>
+  <si>
+    <t>Đổi ngôn ngữ</t>
+  </si>
+  <si>
+    <t>Biên bản họp nhóm ngày 16/10/2014</t>
+  </si>
+  <si>
+    <t>https://ellislab.com/codeigniter/user-guide/general/styleguide.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,16 +154,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -161,11 +199,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -181,10 +344,73 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="A1:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,207 +707,205 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>16</v>
+      <c r="D5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>10</v>
+      <c r="B13" s="7" t="s">
+        <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>18</v>
+        <v>9</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D5:D8"/>
     <mergeCell ref="D9:D12"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="D13:D16"/>
     <mergeCell ref="E13:E16"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="E8:E9"/>
@@ -690,4 +914,248 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="18"/>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="10"/>
+      <c r="F7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>10</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>12</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>13</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="27"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>14</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="27"/>
+      <c r="E18" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="B8:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật kế hoạch
Thêm phần quy trình bảo trì phần mềm
</commit_message>
<xml_diff>
--- a/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
+++ b/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Dự phòng</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>https://ellislab.com/codeigniter/user-guide/general/styleguide.html</t>
+  </si>
+  <si>
+    <t>Cải thiện chức năng tìm kiếm</t>
   </si>
 </sst>
 </file>
@@ -347,28 +350,49 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -379,37 +403,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,24 +719,24 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
@@ -745,16 +748,16 @@
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -762,36 +765,36 @@
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="19"/>
+      <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
     </row>
@@ -799,27 +802,27 @@
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
         <v>15</v>
       </c>
     </row>
@@ -827,36 +830,36 @@
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="19" t="s">
         <v>16</v>
       </c>
     </row>
@@ -864,34 +867,34 @@
       <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -921,7 +924,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -943,23 +946,23 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="26"/>
       <c r="D4" s="5" t="s">
         <v>23</v>
@@ -972,38 +975,38 @@
       <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="27"/>
+      <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="20" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="7"/>
       <c r="F7" t="s">
         <v>35</v>
       </c>
@@ -1012,134 +1015,134 @@
       <c r="A8" s="6">
         <v>4</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="27"/>
+      <c r="C9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="10"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="27"/>
+      <c r="C10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="10"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="11"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>8</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="12"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="9"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>9</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="12"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>10</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>11</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="10"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>12</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>13</v>
       </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="14" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>14</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="10"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
Cập nhật phân tích sự tác động
Đánh số phiếu tiếp nhận
</commit_message>
<xml_diff>
--- a/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
+++ b/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Dự phòng</t>
   </si>
@@ -124,9 +124,6 @@
   </si>
   <si>
     <t>Phuong</t>
-  </si>
-  <si>
-    <t>Đổi ngôn ngữ</t>
   </si>
   <si>
     <t>Biên bản họp nhóm ngày 16/10/2014</t>
@@ -924,7 +921,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,7 +934,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1008,7 +1005,7 @@
       <c r="D7" s="20"/>
       <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1042,9 +1039,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="27"/>
-      <c r="C10" s="14" t="s">
-        <v>33</v>
-      </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="20" t="s">
         <v>32</v>
       </c>
@@ -1139,7 +1134,7 @@
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="7"/>

</xml_diff>

<commit_message>
Cập nhật thứ tự slide báo cáo
Thứ tự báo cáo
Cập nhật biên bản họp nhóm, phân lại các yêu cầu thay đổi
</commit_message>
<xml_diff>
--- a/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
+++ b/BaiTap2/BT01_BT02_BienBanHopNhom20.9.2014.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="34">
   <si>
     <t>Dự phòng</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Giao diện mobile</t>
   </si>
   <si>
-    <t>Phân quyền</t>
-  </si>
-  <si>
     <t>Quản lý đơn vị</t>
   </si>
   <si>
@@ -123,16 +120,13 @@
     <t>Cập nhật tình trạng biến áp</t>
   </si>
   <si>
-    <t>Phuong</t>
-  </si>
-  <si>
     <t>Biên bản họp nhóm ngày 16/10/2014</t>
   </si>
   <si>
-    <t>https://ellislab.com/codeigniter/user-guide/general/styleguide.html</t>
-  </si>
-  <si>
     <t>Cải thiện chức năng tìm kiếm</t>
+  </si>
+  <si>
+    <t>Tiếng Việt</t>
   </si>
 </sst>
 </file>
@@ -328,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -376,6 +370,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -385,12 +385,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -410,6 +404,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,24 +713,24 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="19"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
@@ -745,16 +742,16 @@
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="21" t="s">
         <v>14</v>
       </c>
     </row>
@@ -762,36 +759,36 @@
       <c r="A6" s="4">
         <v>2</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>3</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21" t="s">
         <v>19</v>
       </c>
     </row>
@@ -799,27 +796,27 @@
       <c r="A9" s="4">
         <v>5</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="19"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>6</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
         <v>15</v>
       </c>
     </row>
@@ -827,36 +824,36 @@
       <c r="A11" s="4">
         <v>7</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>8</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>9</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="21" t="s">
         <v>16</v>
       </c>
     </row>
@@ -864,34 +861,34 @@
       <c r="A14" s="4">
         <v>10</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>11</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>12</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -918,10 +915,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,34 +929,34 @@
     <col min="4" max="5" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="18"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="26"/>
       <c r="D4" s="5" t="s">
         <v>23</v>
@@ -968,7 +965,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>1</v>
       </c>
@@ -978,12 +975,16 @@
       <c r="C5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="D5" s="28"/>
       <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>2</v>
       </c>
@@ -991,10 +992,16 @@
       <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
+      <c r="D6" s="29"/>
       <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -1002,13 +1009,16 @@
       <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="20"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="7"/>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>4</v>
       </c>
@@ -1018,10 +1028,16 @@
       <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>5</v>
       </c>
@@ -1029,23 +1045,25 @@
       <c r="C9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="16"/>
+      <c r="E9" s="7"/>
+      <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>6</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="14"/>
-      <c r="D10" s="20" t="s">
-        <v>32</v>
-      </c>
+      <c r="D10" s="17"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>7</v>
       </c>
@@ -1053,45 +1071,69 @@
         <v>6</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="20"/>
+        <v>33</v>
+      </c>
+      <c r="D11" s="17"/>
       <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>8</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="20"/>
+        <v>28</v>
+      </c>
+      <c r="D12" s="17"/>
       <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>9</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="20"/>
+        <v>29</v>
+      </c>
+      <c r="D13" s="17"/>
       <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>10</v>
       </c>
       <c r="B14" s="24"/>
       <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="21"/>
+        <v>30</v>
+      </c>
+      <c r="D14" s="18"/>
       <c r="E14" s="10"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>11</v>
       </c>
@@ -1101,12 +1143,16 @@
       <c r="C15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="25"/>
+      <c r="E15" s="7"/>
+      <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>12</v>
       </c>
@@ -1116,8 +1162,14 @@
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>13</v>
       </c>
@@ -1127,21 +1179,32 @@
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>14</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="7"/>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D10:D14"/>
+  <mergeCells count="10">
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="B11:B14"/>

</xml_diff>